<commit_message>
Removed some hard coded stuff
</commit_message>
<xml_diff>
--- a/test_excel/demo.xlsx
+++ b/test_excel/demo.xlsx
@@ -18,10 +18,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
-    <t>18.0</t>
+    <t>10.0</t>
   </si>
   <si>
-    <t>2.7</t>
+    <t>50.0</t>
   </si>
   <si>
     <t>12.0</t>
@@ -366,7 +366,7 @@
   <dimension ref="H4:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>